<commit_message>
updated rest assured added header map
</commit_message>
<xml_diff>
--- a/src/test/resources/data/sample.xlsx
+++ b/src/test/resources/data/sample.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -66,6 +66,9 @@
   </si>
   <si>
     <t xml:space="preserve">method</t>
+  </si>
+  <si>
+    <t xml:space="preserve">statusCode</t>
   </si>
   <si>
     <t xml:space="preserve">Ahmedabad</t>
@@ -220,9 +223,6 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="13.2295918367347"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -306,16 +306,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
+      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.4591836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -340,28 +344,34 @@
       <c r="G1" s="0" t="s">
         <v>14</v>
       </c>
+      <c r="H1" s="0" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>